<commit_message>
added clear cache before graph building and query performance test
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-tests/engine-it-performance/src/test/resources/datamodel/graph/COMPLEX_1000times.xlsx
+++ b/calculation-engine/engine-tests/engine-it-performance/src/test/resources/datamodel/graph/COMPLEX_1000times.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1005" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="1455" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3357,7 +3357,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>